<commit_message>
add options to influence if and what prefix is used for output
</commit_message>
<xml_diff>
--- a/resources/Numbers.xlsx
+++ b/resources/Numbers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DI_Projects\6\AMS_MI\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DI_Projects\g\utils.powershell-excel-conv\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Three decimals</t>
-  </si>
-  <si>
-    <t>Five decimals</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Show 3 out of 9 decimals</t>
+  </si>
+  <si>
+    <t>Show 5 out of 9 decimals</t>
+  </si>
+  <si>
+    <t>Twelve digit number as nr</t>
+  </si>
+  <si>
+    <t>Twelve digit number standard</t>
+  </si>
+  <si>
+    <t>Eight digit number standard</t>
+  </si>
+  <si>
+    <t>Eleven digit number standard</t>
   </si>
 </sst>
 </file>
@@ -78,10 +90,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -363,34 +376,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C3"/>
+  <dimension ref="B2:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>0.123456789</v>
       </c>
       <c r="C3" s="2">
         <v>0.123456789</v>
+      </c>
+      <c r="D3" s="3">
+        <v>123456789123</v>
+      </c>
+      <c r="E3">
+        <v>123456789123</v>
+      </c>
+      <c r="F3">
+        <v>12345678</v>
+      </c>
+      <c r="G3">
+        <v>12345678912</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>